<commit_message>
feat: (report) create template
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
     <sheet name="permissions" sheetId="10" r:id="rId2"/>
-    <sheet name="branches" sheetId="1" r:id="rId3"/>
-    <sheet name="users" sheetId="8" r:id="rId4"/>
+    <sheet name="programs" sheetId="11" r:id="rId3"/>
+    <sheet name="lecturers" sheetId="12" r:id="rId4"/>
+    <sheet name="marketers" sheetId="13" r:id="rId5"/>
+    <sheet name="students" sheetId="14" r:id="rId6"/>
+    <sheet name="branches" sheetId="1" r:id="rId7"/>
+    <sheet name="users" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -339,13 +343,223 @@
   </si>
   <si>
     <t>Akses Penuh terhadap aplikasi</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
+  <si>
+    <t>KP 2 Anak</t>
+  </si>
+  <si>
+    <t>KP 3 Anak</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>KP 2 Hari</t>
+  </si>
+  <si>
+    <t>KP 2 Hari 2 Anak</t>
+  </si>
+  <si>
+    <t>KP 2 Hari 3 Anak</t>
+  </si>
+  <si>
+    <t>OP 2 Hari</t>
+  </si>
+  <si>
+    <t>KP SA</t>
+  </si>
+  <si>
+    <t>KP SA 2 Anak</t>
+  </si>
+  <si>
+    <t>KP SA 3 Anak</t>
+  </si>
+  <si>
+    <t>OP SA</t>
+  </si>
+  <si>
+    <t>OP 3 Hari</t>
+  </si>
+  <si>
+    <t>OP 3 Hari Ada SA</t>
+  </si>
+  <si>
+    <t>DETAIL</t>
+  </si>
+  <si>
+    <t>Offline Private</t>
+  </si>
+  <si>
+    <t>Offline private 2 Anak</t>
+  </si>
+  <si>
+    <t>Offline Private 3 Anak</t>
+  </si>
+  <si>
+    <t>Online Private</t>
+  </si>
+  <si>
+    <t>Online Reguler</t>
+  </si>
+  <si>
+    <t>Offline 2 Hari</t>
+  </si>
+  <si>
+    <t>Offline 2 hari 2 anak</t>
+  </si>
+  <si>
+    <t>Offline 2 hari 3 anak</t>
+  </si>
+  <si>
+    <t>Online Reguler 2 Hari</t>
+  </si>
+  <si>
+    <t>Offline Private Sabtu Ahad</t>
+  </si>
+  <si>
+    <t>Offline Private Sabtu ahad 2 Anak</t>
+  </si>
+  <si>
+    <t>Offline Private Sabtu ahad 3 anak</t>
+  </si>
+  <si>
+    <t>Online Private Sabtu Ahad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Private 3 Hari </t>
+  </si>
+  <si>
+    <t>Online Private 3 Hari + Sabtu/Ahad</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>01JHC3YCRXPVRG5B009VKVFHC8</t>
+  </si>
+  <si>
+    <t>01JHC3YD0GX123XF20HBXNNC5T</t>
+  </si>
+  <si>
+    <t>01JHC3YD5KKS67SCK1RCAM9BP2</t>
+  </si>
+  <si>
+    <t>01JHC3YDDBX7YP1NQAQ8DG334P</t>
+  </si>
+  <si>
+    <t>01JHC3YDJFEJZHG1CWR2XVDXE6</t>
+  </si>
+  <si>
+    <t>01JHC3YDPDEQZT4BD7ZBHN8151</t>
+  </si>
+  <si>
+    <t>01JHC3YDT9PZJ0J5QDCPWWXWTF</t>
+  </si>
+  <si>
+    <t>01JHC3YDZBZDN5GD2Q8XABHDGC</t>
+  </si>
+  <si>
+    <t>01JHC3YE6687T0QPXNN5GTRKH5</t>
+  </si>
+  <si>
+    <t>01JHC3YEDQSYTWBCKAZK33CGQJ</t>
+  </si>
+  <si>
+    <t>01JHC3YEJ44CGQ6KJ5NVBDTEF3</t>
+  </si>
+  <si>
+    <t>01JHC3YEQ6S7CQ2VRV8FE2HM0P</t>
+  </si>
+  <si>
+    <t>01JHC3YEWYHKF88XQAEF9Z9CCS</t>
+  </si>
+  <si>
+    <t>01JHC3YF0XQT8NFWSTNCJ05JHM</t>
+  </si>
+  <si>
+    <t>01JHC3YF6QE559NX3HEYDHSNVT</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>Andi</t>
+  </si>
+  <si>
+    <t>Bayu</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Ayu</t>
+  </si>
+  <si>
+    <t>Bendy</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Arya</t>
+  </si>
+  <si>
+    <t>Burhan</t>
+  </si>
+  <si>
+    <t>Cahya</t>
+  </si>
+  <si>
+    <t>IDENTIFIER</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>01JHC94X3Y69KQ3C6BTBA70E24</t>
+  </si>
+  <si>
+    <t>01JHC94XA8KQT1EPF72ARYBB0R</t>
+  </si>
+  <si>
+    <t>01JHC94XHY8S14XP56KEX15WFT</t>
+  </si>
+  <si>
+    <t>01JHC9Q9THQDN6XMEP5NKFXY01</t>
+  </si>
+  <si>
+    <t>01JHC9QA4FR6NB9GGATVMYCVFD</t>
+  </si>
+  <si>
+    <t>01JHC9QAATNGNMKW10RR9R6M0F</t>
+  </si>
+  <si>
+    <t>01JHC9RM7T7VPJQS8GD36AAHJH</t>
+  </si>
+  <si>
+    <t>01JHC9RMBQD604WB2SE6P8D899</t>
+  </si>
+  <si>
+    <t>01JHC9RMFEGFEMNRMWHC0GST9J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +601,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -411,7 +632,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
@@ -420,6 +641,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,13 +932,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="29.765625"/>
-    <col customWidth="true" max="2" min="2" width="13.921875"/>
+    <col min="1" max="1" width="29.765625" customWidth="1"/>
+    <col min="2" max="2" width="13.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -723,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -731,7 +954,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -739,7 +962,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -747,7 +970,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -755,7 +978,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -772,16 +995,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6F55B8-A7A9-440E-B0B3-34A2186B3EA3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="3" min="3" width="26.765625"/>
+    <col min="3" max="3" width="26.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -792,7 +1015,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -809,11 +1032,426 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C81C74-3587-48B7-ABC1-5079A3AD0FF2}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="30.23046875"/>
+    <col customWidth="true" max="2" min="2" width="15.765625"/>
+    <col customWidth="true" max="3" min="3" width="25.15234375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="5">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1070000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1420000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="5">
+        <v>675000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="5">
+        <v>475000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="5">
+        <v>595000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="5">
+        <v>885000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1170000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="5">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="5">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="5">
+        <v>970000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1220000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="5">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="5">
+        <v>550000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="5">
+        <v>620000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup r:id="rId1" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF89C235-C296-48F6-99FC-8FE712EEFFDA}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24984F5D-3F97-466A-8F2C-FC15FC3B328C}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C681E41-5EC2-4E8F-9FDC-93FC7C835BBE}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col customWidth="true" max="2" min="2" width="11.3046875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -843,7 +1481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672936D5-D2E7-4DCD-8047-B176548ED4E4}">
   <dimension ref="A1:G20"/>
   <sheetViews>

</xml_diff>

<commit_message>
refactor: (report) create and update add days of meetings
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="5"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="180">
   <si>
     <t>ID</t>
   </si>
@@ -553,6 +553,24 @@
   </si>
   <si>
     <t>01JHC9RMFEGFEMNRMWHC0GST9J</t>
+  </si>
+  <si>
+    <t>DAYS</t>
+  </si>
+  <si>
+    <t>1|3|5</t>
+  </si>
+  <si>
+    <t>1|3</t>
+  </si>
+  <si>
+    <t>6|7</t>
+  </si>
+  <si>
+    <t>1|2|3|4|5</t>
+  </si>
+  <si>
+    <t>5|6|7</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C81C74-3587-48B7-ABC1-5079A3AD0FF2}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1044,9 +1062,10 @@
     <col customWidth="true" max="1" min="1" width="30.23046875"/>
     <col customWidth="true" max="2" min="2" width="15.765625"/>
     <col customWidth="true" max="3" min="3" width="25.15234375"/>
+    <col customWidth="true" max="5" min="5" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1059,8 +1078,11 @@
       <c r="D1" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -1073,8 +1095,11 @@
       <c r="D2" s="5">
         <v>720000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -1087,8 +1112,11 @@
       <c r="D3" s="5">
         <v>1070000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1101,8 +1129,11 @@
       <c r="D4" s="5">
         <v>1420000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1115,8 +1146,11 @@
       <c r="D5" s="5">
         <v>675000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1129,8 +1163,11 @@
       <c r="D6" s="5">
         <v>475000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1143,8 +1180,11 @@
       <c r="D7" s="5">
         <v>595000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1157,8 +1197,11 @@
       <c r="D8" s="5">
         <v>885000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -1171,8 +1214,11 @@
       <c r="D9" s="5">
         <v>1170000</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -1185,8 +1231,11 @@
       <c r="D10" s="5">
         <v>450000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1199,8 +1248,11 @@
       <c r="D11" s="5">
         <v>720000</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -1213,8 +1265,11 @@
       <c r="D12" s="5">
         <v>970000</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -1227,8 +1282,11 @@
       <c r="D13" s="5">
         <v>1220000</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -1241,8 +1299,11 @@
       <c r="D14" s="5">
         <v>600000</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -1255,8 +1316,11 @@
       <c r="D15" s="5">
         <v>550000</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1268,6 +1332,9 @@
       </c>
       <c r="D16" s="5">
         <v>620000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1284,9 +1351,9 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1367,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -1308,7 +1375,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1316,7 +1383,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -1337,9 +1404,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1353,7 +1420,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -1361,7 +1428,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1369,7 +1436,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -1386,16 +1453,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C681E41-5EC2-4E8F-9FDC-93FC7C835BBE}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="2" min="2" width="11.3046875"/>
+    <col min="2" max="2" width="11.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1475,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1419,7 +1486,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>166</v>
       </c>
@@ -1430,7 +1497,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
chore: implement seeding for student managers and update marketers to include student_manager_id
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\freelance\kaffapriority-finance\db\seeds\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677CC3B6-E623-4C95-B10D-5DFE8D0408CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
     <sheet name="permissions" sheetId="10" r:id="rId2"/>
     <sheet name="programs" sheetId="11" r:id="rId3"/>
     <sheet name="lecturers" sheetId="12" r:id="rId4"/>
-    <sheet name="marketers" sheetId="13" r:id="rId5"/>
-    <sheet name="students" sheetId="14" r:id="rId6"/>
-    <sheet name="branches" sheetId="1" r:id="rId7"/>
-    <sheet name="users" sheetId="8" r:id="rId8"/>
+    <sheet name="student_managers" sheetId="15" r:id="rId5"/>
+    <sheet name="marketers" sheetId="13" r:id="rId6"/>
+    <sheet name="students" sheetId="14" r:id="rId7"/>
+    <sheet name="branches" sheetId="1" r:id="rId8"/>
+    <sheet name="users" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -571,13 +573,25 @@
   </si>
   <si>
     <t>5|6|7</t>
+  </si>
+  <si>
+    <t>Ayu manager</t>
+  </si>
+  <si>
+    <t>Bendy manager</t>
+  </si>
+  <si>
+    <t>Clara manager</t>
+  </si>
+  <si>
+    <t>STUDENT_MANAGER_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,7 +626,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -652,24 +666,24 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 2 10" xfId="2"/>
-    <cellStyle name="Normal 83 3 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 83 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -682,7 +696,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1053,19 +1067,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C81C74-3587-48B7-ABC1-5079A3AD0FF2}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="30.23046875"/>
-    <col customWidth="true" max="2" min="2" width="15.765625"/>
-    <col customWidth="true" max="3" min="3" width="25.15234375"/>
-    <col customWidth="true" max="5" min="5" width="10"/>
+    <col min="1" max="1" width="30.23046875" customWidth="1"/>
+    <col min="2" max="2" width="15.765625" customWidth="1"/>
+    <col min="3" max="3" width="25.15234375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1096,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -1099,7 +1113,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -1116,7 +1130,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1133,7 +1147,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1150,7 +1164,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1167,7 +1181,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1184,7 +1198,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1201,7 +1215,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -1218,7 +1232,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -1235,7 +1249,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1252,7 +1266,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -1269,7 +1283,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -1286,7 +1300,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -1303,7 +1317,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -1320,7 +1334,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1339,7 +1353,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup r:id="rId1" orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1397,14 +1411,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24984F5D-3F97-466A-8F2C-FC15FC3B328C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7B50C7-BA36-4D59-952C-93BFF70EB2FF}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="33.4609375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
@@ -1425,7 +1442,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -1433,7 +1450,7 @@
         <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -1441,7 +1458,7 @@
         <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1450,6 +1467,66 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24984F5D-3F97-466A-8F2C-FC15FC3B328C}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="30.765625" customWidth="1"/>
+    <col min="2" max="2" width="32.3828125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C681E41-5EC2-4E8F-9FDC-93FC7C835BBE}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1513,7 +1590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1548,7 +1625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672936D5-D2E7-4DCD-8047-B176548ED4E4}">
   <dimension ref="A1:G20"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: (master) add student manager fields to marketers and implement seeding for student managers
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\freelance\kaffapriority-finance\db\seeds\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677CC3B6-E623-4C95-B10D-5DFE8D0408CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -585,13 +584,22 @@
   </si>
   <si>
     <t>STUDENT_MANAGER_ID</t>
+  </si>
+  <si>
+    <t>01JJ0MYHTBXSDAF5Q86782Q4F7</t>
+  </si>
+  <si>
+    <t>01JJ0MYHYSEF1M8Q5QHS979009</t>
+  </si>
+  <si>
+    <t>01JJ0MYJ24BYMQFJCXQCBREQE8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,7 +634,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -666,24 +674,24 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 2 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 83 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 10" xfId="2"/>
+    <cellStyle name="Normal 83 3 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -696,7 +704,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -964,13 +972,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="29.765625" customWidth="1"/>
-    <col min="2" max="2" width="13.921875" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="29.765625"/>
+    <col customWidth="true" max="2" min="2" width="13.921875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -978,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -986,7 +994,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -994,7 +1002,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1002,7 +1010,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -1010,7 +1018,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1365,9 +1373,9 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1389,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -1389,7 +1397,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1397,7 +1405,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -1418,12 +1426,12 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="33.4609375" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="33.4609375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1445,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -1445,7 +1453,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -1470,17 +1478,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24984F5D-3F97-466A-8F2C-FC15FC3B328C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="30.765625" customWidth="1"/>
-    <col min="2" max="2" width="32.3828125" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="30.765625"/>
+    <col customWidth="true" max="2" min="2" width="32.3828125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1505,10 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
       <c r="B2" t="s">
         <v>171</v>
       </c>
@@ -1505,7 +1516,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
       <c r="B3" t="s">
         <v>172</v>
       </c>
@@ -1513,7 +1527,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
       <c r="B4" t="s">
         <v>173</v>
       </c>
@@ -1534,12 +1551,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="2" max="2" width="11.3046875" customWidth="1"/>
+    <col customWidth="true" max="2" min="2" width="11.3046875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1552,7 +1569,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1563,7 +1580,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>166</v>
       </c>
@@ -1574,7 +1591,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
feat: (master) add commission_fee and lecturer_fee to programs table and update related seed and entity logic
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
@@ -22,17 +22,28 @@
     <sheet name="branches" sheetId="1" r:id="rId8"/>
     <sheet name="users" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -593,6 +604,12 @@
   </si>
   <si>
     <t>01JJ0MYJ24BYMQFJCXQCBREQE8</t>
+  </si>
+  <si>
+    <t>COMMISSION FEE</t>
+  </si>
+  <si>
+    <t>LECTURER FEE</t>
   </si>
 </sst>
 </file>
@@ -672,7 +689,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
@@ -683,6 +700,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,13 +991,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="29.765625"/>
-    <col customWidth="true" max="2" min="2" width="13.921875"/>
+    <col min="1" max="1" width="29.765625" customWidth="1"/>
+    <col min="2" max="2" width="13.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -986,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -994,7 +1013,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1002,7 +1021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1010,7 +1029,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -1018,7 +1037,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1073,21 +1092,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C81C74-3587-48B7-ABC1-5079A3AD0FF2}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="30.23046875" customWidth="1"/>
-    <col min="2" max="2" width="15.765625" customWidth="1"/>
-    <col min="3" max="3" width="25.15234375" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="30.23046875"/>
+    <col customWidth="true" max="2" min="2" width="15.765625"/>
+    <col customWidth="true" max="3" min="3" width="25.15234375"/>
+    <col customWidth="true" max="5" min="5" width="10"/>
+    <col customWidth="true" max="6" min="6" width="15.61328125"/>
+    <col customWidth="true" max="7" min="7" width="14.4609375"/>
+    <col customWidth="true" max="8" min="8" width="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1103,8 +1125,15 @@
       <c r="E1" s="3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -1120,8 +1149,15 @@
       <c r="E2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F2" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="6">
+        <v>485000</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -1137,8 +1173,15 @@
       <c r="E3" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3" s="6">
+        <v>200000</v>
+      </c>
+      <c r="G3" s="6">
+        <v>725000</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1154,8 +1197,15 @@
       <c r="E4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4" s="6">
+        <v>300000</v>
+      </c>
+      <c r="G4" s="6">
+        <v>965000</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -1171,8 +1221,15 @@
       <c r="E5" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="6">
+        <v>440000</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1188,8 +1245,15 @@
       <c r="E6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="6">
+        <v>240000</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1205,8 +1269,15 @@
       <c r="E7" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="6">
+        <v>360000</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1222,8 +1293,15 @@
       <c r="E8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F8" s="6">
+        <v>200000</v>
+      </c>
+      <c r="G8" s="6">
+        <v>540000</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -1239,8 +1317,15 @@
       <c r="E9" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9" s="6">
+        <v>300000</v>
+      </c>
+      <c r="G9" s="6">
+        <v>715000</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -1256,8 +1341,15 @@
       <c r="E10" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F10" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="6">
+        <v>215000</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1273,8 +1365,15 @@
       <c r="E11" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F11" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G11" s="6">
+        <v>485000</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -1290,8 +1389,15 @@
       <c r="E12" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F12" s="6">
+        <v>200000</v>
+      </c>
+      <c r="G12" s="6">
+        <v>625000</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -1307,8 +1413,15 @@
       <c r="E13" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F13" s="6">
+        <v>300000</v>
+      </c>
+      <c r="G13" s="6">
+        <v>765000</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -1324,8 +1437,15 @@
       <c r="E14" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F14" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="6">
+        <v>365000</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -1341,8 +1461,15 @@
       <c r="E15" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F15" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="6">
+        <v>315000</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1358,10 +1485,17 @@
       <c r="E16" t="s">
         <v>179</v>
       </c>
+      <c r="F16" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G16" s="6">
+        <v>385000</v>
+      </c>
+      <c r="H16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup r:id="rId1" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1373,9 +1507,9 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1523,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -1397,7 +1531,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -1405,7 +1539,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -1426,12 +1560,12 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="33.4609375"/>
+    <col min="1" max="1" width="33.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1579,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -1453,7 +1587,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1461,7 +1595,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -1478,17 +1612,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24984F5D-3F97-466A-8F2C-FC15FC3B328C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView topLeftCell="AH1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="30.765625"/>
-    <col customWidth="true" max="2" min="2" width="32.3828125"/>
+    <col min="1" max="1" width="30.765625" customWidth="1"/>
+    <col min="2" max="2" width="32.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1639,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -1516,7 +1650,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -1527,7 +1661,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -1551,12 +1685,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="true" max="2" min="2" width="11.3046875"/>
+    <col min="2" max="2" width="11.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1703,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1580,7 +1714,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>166</v>
       </c>
@@ -1591,7 +1725,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
feat: (report) enhance GetRegistrationListPerLecturer request with lecturer and student ID filters
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -991,13 +991,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="29.765625" customWidth="1"/>
-    <col min="2" max="2" width="13.921875" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="29.765625"/>
+    <col customWidth="true" max="2" min="2" width="13.921875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>100</v>
       </c>

</xml_diff>